<commit_message>
Excel: update to exchange rates
</commit_message>
<xml_diff>
--- a/ms-office/Export Factory.xlsx
+++ b/ms-office/Export Factory.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -12,7 +12,7 @@
     <sheet name="Exchange Rate" sheetId="4" r:id="rId3"/>
     <sheet name="Profit and Loss" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -169,6 +169,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -216,7 +219,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -251,7 +254,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -471,7 +474,7 @@
     <col min="1" max="1" width="15.42578125" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" style="5" customWidth="1"/>
     <col min="3" max="3" width="14" style="6" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -501,7 +504,7 @@
       </c>
       <c r="D3" s="3">
         <f>B3/VLOOKUP(C3,'Exchange Rate'!$A:$B,2,FALSE)</f>
-        <v>32051.282051282051</v>
+        <v>29954.110303015783</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -531,7 +534,7 @@
       </c>
       <c r="D5" s="3">
         <f>B5/VLOOKUP(C5,'Exchange Rate'!$A:$B,2,FALSE)</f>
-        <v>8695.652173913044</v>
+        <v>8005.9564315851003</v>
       </c>
     </row>
   </sheetData>
@@ -544,7 +547,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,7 +600,7 @@
       </c>
       <c r="D4" s="3">
         <f>B4/VLOOKUP(C4,'Exchange Rate'!$A:$B,2,FALSE)</f>
-        <v>12658.227848101265</v>
+        <v>11148.334160168117</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -627,7 +630,7 @@
       </c>
       <c r="D6" s="3">
         <f>B6/VLOOKUP(C6,'Exchange Rate'!$A:$B,2,FALSE)</f>
-        <v>26086.956521739132</v>
+        <v>24017.869294755299</v>
       </c>
     </row>
   </sheetData>
@@ -641,7 +644,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,7 +666,7 @@
         <v>15</v>
       </c>
       <c r="B3">
-        <v>1.58</v>
+        <v>1.79399</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -671,7 +674,7 @@
         <v>19</v>
       </c>
       <c r="B4">
-        <v>1.1499999999999999</v>
+        <v>1.2490699999999999</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -687,7 +690,7 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <v>1.56</v>
+        <v>1.6692199999999999</v>
       </c>
     </row>
   </sheetData>
@@ -695,6 +698,7 @@
     <sortCondition ref="A3"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -703,7 +707,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,15 +732,15 @@
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <f>SUM(Income!D:D)</f>
-        <v>60746.934225195087</v>
+        <v>57960.066734600885</v>
       </c>
       <c r="B3" s="3">
         <f>SUM(Costs!D:D)</f>
-        <v>73745.184369840397</v>
+        <v>70166.203454923409</v>
       </c>
       <c r="C3" s="9">
         <f>A3-B3</f>
-        <v>-12998.25014464531</v>
+        <v>-12206.136720322524</v>
       </c>
     </row>
   </sheetData>

</xml_diff>